<commit_message>
final commit before demo
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sandesh Velhal\eclipse-workspace\Servicenow-AllModule\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7814C70E-E347-4A15-95D3-7D3BE70C08A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF77C7F6-DCC1-4AB7-A03A-0B4338125305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{47AEF9C5-A68B-4616-944B-F17818BC6EA4}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="3" xr2:uid="{47AEF9C5-A68B-4616-944B-F17818BC6EA4}"/>
   </bookViews>
   <sheets>
     <sheet name="ImpersonateUser" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>User</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>add value</t>
-  </si>
-  <si>
     <t>Assignment group</t>
   </si>
   <si>
@@ -201,6 +198,21 @@
   </si>
   <si>
     <t>Beth Anglin</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>2 - High</t>
+  </si>
+  <si>
+    <t>Error Pop Up</t>
+  </si>
+  <si>
+    <t>The following mandatory fields are not filled in: Problem statement</t>
+  </si>
+  <si>
+    <t>Impersonate user</t>
   </si>
 </sst>
 </file>
@@ -264,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -276,6 +288,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,7 +607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4232BF5-167B-438D-AD11-4378C7AE8B69}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -605,7 +620,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -637,10 +652,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -712,22 +727,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
       <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
-        <v>38</v>
-      </c>
       <c r="H1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -763,10 +778,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DB1441-C323-479D-A628-08A5A45D8D8F}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -785,170 +800,200 @@
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1"/>
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
+      <c r="A3" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="28.55" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1"/>
+      <c r="A12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>34</v>
+      <c r="A14" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="28.55" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>42</v>
+      <c r="A20" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="28.55" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>44</v>
+      <c r="A22" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.95" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1020,27 +1065,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
-        <v>55</v>
-      </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>